<commit_message>
v2.0 new release after Revision
Changes in the new release:
- improved input data including demands, investment information, hydrogen production cost
- variable transport media for ship transport can now be defined through commodity column
- code partly reoganized and cleaned
- bug fixing
</commit_message>
<xml_diff>
--- a/data/data_output/properties_table_transport.xlsx
+++ b/data/data_output/properties_table_transport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oliver\Documents\RUB\02_Promotion\Aggregierung von erneuerbaren Potentialen und Energieinfrastruktur\StEAM_h2_transport v1_0\data\data_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDCDE3F-27E1-43C4-A13E-AE63C72AB3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA6EEE3-430B-457F-9AB5-E143FBC852DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7140" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-4725" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="15" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="Input Table" sheetId="13" r:id="rId4"/>
     <sheet name="Quellen" sheetId="12" r:id="rId5"/>
     <sheet name="properties_table" sheetId="20" r:id="rId6"/>
-    <sheet name="properties_table bkp" sheetId="17" r:id="rId7"/>
-    <sheet name="terminal recherche" sheetId="18" r:id="rId8"/>
-    <sheet name="reports" sheetId="21" r:id="rId9"/>
+    <sheet name="properties_table bkp (2)" sheetId="22" r:id="rId7"/>
+    <sheet name="properties_table bkp" sheetId="17" r:id="rId8"/>
+    <sheet name="terminal recherche" sheetId="18" r:id="rId9"/>
+    <sheet name="reports" sheetId="21" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nodes!$A$1:$J$1</definedName>
@@ -269,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3696" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3737" uniqueCount="737">
   <si>
     <t>CCGT</t>
   </si>
@@ -2457,6 +2458,33 @@
   </si>
   <si>
     <t>node_slack_pos</t>
+  </si>
+  <si>
+    <t>node_h2</t>
+  </si>
+  <si>
+    <t>terminal connection</t>
+  </si>
+  <si>
+    <t>ship connection</t>
+  </si>
+  <si>
+    <t>pipeline connection</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>node / none</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>continuous</t>
   </si>
 </sst>
 </file>
@@ -2467,7 +2495,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2532,6 +2560,11 @@
       <color theme="1"/>
       <name val="CMU Serif"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="CMU Serif"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2561,7 +2594,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2591,19 +2624,31 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -13304,6 +13349,225 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BC4F0D-8ECD-49DD-8015-689C8EFF3A6E}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" t="s">
+        <v>713</v>
+      </c>
+      <c r="C1" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1" t="s">
+        <v>715</v>
+      </c>
+      <c r="E1" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>712</v>
+      </c>
+      <c r="B2" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2" t="s">
+        <v>714</v>
+      </c>
+      <c r="D2" t="s">
+        <v>715</v>
+      </c>
+      <c r="E2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>712</v>
+      </c>
+      <c r="B3" t="s">
+        <v>713</v>
+      </c>
+      <c r="C3" t="s">
+        <v>714</v>
+      </c>
+      <c r="D3" t="s">
+        <v>715</v>
+      </c>
+      <c r="E3" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>712</v>
+      </c>
+      <c r="B4" t="s">
+        <v>713</v>
+      </c>
+      <c r="C4" t="s">
+        <v>714</v>
+      </c>
+      <c r="D4" t="s">
+        <v>715</v>
+      </c>
+      <c r="E4" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>712</v>
+      </c>
+      <c r="B5" t="s">
+        <v>713</v>
+      </c>
+      <c r="C5" t="s">
+        <v>714</v>
+      </c>
+      <c r="D5" t="s">
+        <v>715</v>
+      </c>
+      <c r="E5" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>712</v>
+      </c>
+      <c r="B6" t="s">
+        <v>713</v>
+      </c>
+      <c r="C6" t="s">
+        <v>714</v>
+      </c>
+      <c r="D6" t="s">
+        <v>715</v>
+      </c>
+      <c r="E6" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>712</v>
+      </c>
+      <c r="B7" t="s">
+        <v>713</v>
+      </c>
+      <c r="C7" t="s">
+        <v>714</v>
+      </c>
+      <c r="D7" t="s">
+        <v>715</v>
+      </c>
+      <c r="E7" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>712</v>
+      </c>
+      <c r="B8" t="s">
+        <v>713</v>
+      </c>
+      <c r="C8" t="s">
+        <v>714</v>
+      </c>
+      <c r="D8" t="s">
+        <v>715</v>
+      </c>
+      <c r="E8" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>712</v>
+      </c>
+      <c r="B9" t="s">
+        <v>713</v>
+      </c>
+      <c r="C9" t="s">
+        <v>714</v>
+      </c>
+      <c r="D9" t="s">
+        <v>715</v>
+      </c>
+      <c r="E9" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>712</v>
+      </c>
+      <c r="B10" t="s">
+        <v>713</v>
+      </c>
+      <c r="C10" t="s">
+        <v>714</v>
+      </c>
+      <c r="D10" t="s">
+        <v>715</v>
+      </c>
+      <c r="E10" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>712</v>
+      </c>
+      <c r="B11" t="s">
+        <v>713</v>
+      </c>
+      <c r="C11" t="s">
+        <v>714</v>
+      </c>
+      <c r="D11" t="s">
+        <v>715</v>
+      </c>
+      <c r="E11" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>712</v>
+      </c>
+      <c r="B12" t="s">
+        <v>713</v>
+      </c>
+      <c r="C12" t="s">
+        <v>714</v>
+      </c>
+      <c r="D12" t="s">
+        <v>715</v>
+      </c>
+      <c r="E12" t="s">
+        <v>727</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66838D55-9326-46D6-AA2D-627081A9FDEE}">
   <dimension ref="A1:F577"/>
@@ -38711,10 +38975,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F14987-88B9-4634-831B-7CF8238BAB8C}">
-  <dimension ref="B2:W26"/>
+  <dimension ref="B2:W23"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38732,58 +38996,58 @@
       <c r="B2" s="10" t="s">
         <v>711</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>363</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>698</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="14" t="s">
         <v>367</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="T2" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="14" t="s">
         <v>367</v>
       </c>
       <c r="W2" s="17"/>
@@ -38792,26 +39056,26 @@
       <c r="B3" s="11" t="s">
         <v>702</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="15"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="14"/>
       <c r="W3" s="17"/>
     </row>
     <row r="4" spans="2:23" ht="15.5" x14ac:dyDescent="0.45">
@@ -39150,67 +39414,67 @@
       <c r="B13" s="10" t="s">
         <v>704</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>706</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>707</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>708</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
     </row>
     <row r="14" spans="2:23" ht="74" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
     </row>
     <row r="15" spans="2:23" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B15" s="14" t="s">
-        <v>352</v>
+      <c r="B15" s="18" t="s">
+        <v>699</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>82</v>
@@ -39227,7 +39491,7 @@
       <c r="J15" s="12"/>
     </row>
     <row r="16" spans="2:23" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B16" s="14"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="11"/>
       <c r="D16" s="12" t="s">
         <v>82</v>
@@ -39242,7 +39506,7 @@
       <c r="J16" s="12"/>
     </row>
     <row r="17" spans="2:11" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B17" s="14"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12" t="s">
@@ -39257,8 +39521,8 @@
       <c r="J17" s="12"/>
     </row>
     <row r="18" spans="2:11" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B18" s="14" t="s">
-        <v>699</v>
+      <c r="B18" s="18" t="s">
+        <v>700</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>82</v>
@@ -39275,7 +39539,7 @@
       <c r="J18" s="12"/>
     </row>
     <row r="19" spans="2:11" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B19" s="14"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="11"/>
       <c r="D19" s="12" t="s">
         <v>82</v>
@@ -39290,7 +39554,7 @@
       <c r="J19" s="12"/>
     </row>
     <row r="20" spans="2:11" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B20" s="14"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12" t="s">
@@ -39305,8 +39569,8 @@
       <c r="J20" s="12"/>
     </row>
     <row r="21" spans="2:11" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B21" s="14" t="s">
-        <v>700</v>
+      <c r="B21" s="18" t="s">
+        <v>701</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>82</v>
@@ -39322,75 +39586,52 @@
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="2:11" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="14"/>
-      <c r="C22" s="11"/>
+    <row r="22" spans="2:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="18"/>
       <c r="D22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="11"/>
       <c r="F22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="2:11" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B23" s="14"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="2:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="18"/>
       <c r="E23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
       <c r="H23" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="2:11" ht="15.5" x14ac:dyDescent="0.45">
-      <c r="B24" s="14" t="s">
-        <v>701</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="2:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B25" s="14"/>
-      <c r="D25" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="2:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="14"/>
-      <c r="E26" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>82</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="41">
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="G2:H3"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="F13:F14"/>
@@ -39404,35 +39645,9 @@
     <mergeCell ref="M13:M14"/>
     <mergeCell ref="K13:K14"/>
     <mergeCell ref="L13:L14"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="Q13:Q14"/>
     <mergeCell ref="P13:P14"/>
-    <mergeCell ref="R2:R3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="E2:F3"/>
-    <mergeCell ref="G2:H3"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39440,11 +39655,240 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925A240D-5DE8-47D8-BA8D-2349C3F5F6D5}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="93" x14ac:dyDescent="0.4">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>731</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>729</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A2" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>734</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A3" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A4" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A5" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A6" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>733</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>733</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A7" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A8" s="21" t="s">
+        <v>351</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.4">
+      <c r="A9" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A10" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28" x14ac:dyDescent="0.4">
+      <c r="A11" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28" x14ac:dyDescent="0.4">
+      <c r="A12" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28" x14ac:dyDescent="0.4">
+      <c r="A13" s="22" t="s">
+        <v>369</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19" t="s">
+        <v>736</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>736</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+      <c r="A14" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC04917-52AF-4438-A91F-52D987D1A7EF}">
   <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:X8"/>
+      <selection sqref="A1:X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -39821,7 +40265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14C2600-D565-460B-85F0-CFCEB42823E9}">
   <dimension ref="A1:T92"/>
   <sheetViews>
@@ -41571,223 +42015,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BC4F0D-8ECD-49DD-8015-689C8EFF3A6E}">
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>712</v>
-      </c>
-      <c r="B1" t="s">
-        <v>713</v>
-      </c>
-      <c r="C1" t="s">
-        <v>714</v>
-      </c>
-      <c r="D1" t="s">
-        <v>715</v>
-      </c>
-      <c r="E1" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>712</v>
-      </c>
-      <c r="B2" t="s">
-        <v>713</v>
-      </c>
-      <c r="C2" t="s">
-        <v>714</v>
-      </c>
-      <c r="D2" t="s">
-        <v>715</v>
-      </c>
-      <c r="E2" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>712</v>
-      </c>
-      <c r="B3" t="s">
-        <v>713</v>
-      </c>
-      <c r="C3" t="s">
-        <v>714</v>
-      </c>
-      <c r="D3" t="s">
-        <v>715</v>
-      </c>
-      <c r="E3" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>712</v>
-      </c>
-      <c r="B4" t="s">
-        <v>713</v>
-      </c>
-      <c r="C4" t="s">
-        <v>714</v>
-      </c>
-      <c r="D4" t="s">
-        <v>715</v>
-      </c>
-      <c r="E4" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>712</v>
-      </c>
-      <c r="B5" t="s">
-        <v>713</v>
-      </c>
-      <c r="C5" t="s">
-        <v>714</v>
-      </c>
-      <c r="D5" t="s">
-        <v>715</v>
-      </c>
-      <c r="E5" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>712</v>
-      </c>
-      <c r="B6" t="s">
-        <v>713</v>
-      </c>
-      <c r="C6" t="s">
-        <v>714</v>
-      </c>
-      <c r="D6" t="s">
-        <v>715</v>
-      </c>
-      <c r="E6" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>712</v>
-      </c>
-      <c r="B7" t="s">
-        <v>713</v>
-      </c>
-      <c r="C7" t="s">
-        <v>714</v>
-      </c>
-      <c r="D7" t="s">
-        <v>715</v>
-      </c>
-      <c r="E7" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>712</v>
-      </c>
-      <c r="B8" t="s">
-        <v>713</v>
-      </c>
-      <c r="C8" t="s">
-        <v>714</v>
-      </c>
-      <c r="D8" t="s">
-        <v>715</v>
-      </c>
-      <c r="E8" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>712</v>
-      </c>
-      <c r="B9" t="s">
-        <v>713</v>
-      </c>
-      <c r="C9" t="s">
-        <v>714</v>
-      </c>
-      <c r="D9" t="s">
-        <v>715</v>
-      </c>
-      <c r="E9" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>712</v>
-      </c>
-      <c r="B10" t="s">
-        <v>713</v>
-      </c>
-      <c r="C10" t="s">
-        <v>714</v>
-      </c>
-      <c r="D10" t="s">
-        <v>715</v>
-      </c>
-      <c r="E10" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>712</v>
-      </c>
-      <c r="B11" t="s">
-        <v>713</v>
-      </c>
-      <c r="C11" t="s">
-        <v>714</v>
-      </c>
-      <c r="D11" t="s">
-        <v>715</v>
-      </c>
-      <c r="E11" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>712</v>
-      </c>
-      <c r="B12" t="s">
-        <v>713</v>
-      </c>
-      <c r="C12" t="s">
-        <v>714</v>
-      </c>
-      <c r="D12" t="s">
-        <v>715</v>
-      </c>
-      <c r="E12" t="s">
-        <v>727</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>